<commit_message>
Addded a Hangout session to the agenda of the kick-off meeting
</commit_message>
<xml_diff>
--- a/Meetings/kick-off meeting/Bioinformatics_initiative_kick-off_agenda_draft.xlsx
+++ b/Meetings/kick-off meeting/Bioinformatics_initiative_kick-off_agenda_draft.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Lunch</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Summary and Discussion</t>
+  </si>
+  <si>
+    <t>Hangout</t>
   </si>
 </sst>
 </file>
@@ -262,43 +265,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,7 +606,7 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +627,7 @@
     <row r="2" spans="2:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
-      <c r="C3" s="31">
+      <c r="C3" s="20">
         <v>42338</v>
       </c>
       <c r="D3" s="17" t="s">
@@ -654,7 +657,9 @@
       <c r="C5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="28" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="9">
         <v>0.41666666666666702</v>
       </c>
@@ -668,13 +673,13 @@
       <c r="B6" s="9">
         <v>0.4375</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="9">
         <v>0.4375</v>
       </c>
       <c r="H6"/>
-      <c r="I6" s="27"/>
+      <c r="I6" s="32"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -693,7 +698,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="H7"/>
-      <c r="I7" s="27"/>
+      <c r="I7" s="32"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -705,13 +710,13 @@
       <c r="C8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="29"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="9">
         <v>0.47916666666666669</v>
       </c>
       <c r="H8"/>
       <c r="I8" s="19"/>
-      <c r="J8" s="27"/>
+      <c r="J8" s="32"/>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
@@ -720,14 +725,14 @@
       <c r="B9" s="9">
         <v>0.5</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="30"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="9">
         <v>0.5</v>
       </c>
       <c r="H9"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
       <c r="K9"/>
       <c r="L9" s="19"/>
       <c r="M9"/>
@@ -736,17 +741,17 @@
       <c r="B10" s="9">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="24" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="9">
         <v>0.52083333333333337</v>
       </c>
       <c r="H10"/>
-      <c r="I10" s="27"/>
+      <c r="I10" s="32"/>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" s="19"/>
@@ -756,13 +761,13 @@
       <c r="B11" s="9">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="9">
         <v>0.54166666666666696</v>
       </c>
       <c r="H11"/>
-      <c r="I11" s="27"/>
+      <c r="I11" s="32"/>
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" s="19"/>
@@ -773,16 +778,16 @@
       <c r="B12" s="9">
         <v>0.5625</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="9">
         <v>0.5625</v>
       </c>
       <c r="H12"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
       <c r="K12"/>
-      <c r="L12" s="27"/>
+      <c r="L12" s="32"/>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
     </row>
@@ -790,18 +795,18 @@
       <c r="B13" s="9">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="24"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="9">
         <v>0.58333333333333337</v>
       </c>
       <c r="H13"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
       <c r="K13"/>
-      <c r="L13" s="27"/>
+      <c r="L13" s="32"/>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
     </row>
@@ -809,16 +814,16 @@
       <c r="B14" s="9">
         <v>0.60416666666666663</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="9">
         <v>0.60416666666666663</v>
       </c>
       <c r="H14"/>
       <c r="I14" s="19"/>
-      <c r="J14" s="27"/>
+      <c r="J14" s="32"/>
       <c r="K14"/>
-      <c r="L14" s="27"/>
+      <c r="L14" s="32"/>
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
     </row>
@@ -826,16 +831,16 @@
       <c r="B15" s="9">
         <v>0.625</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="9">
         <v>0.625</v>
       </c>
       <c r="H15"/>
       <c r="I15" s="19"/>
-      <c r="J15" s="27"/>
+      <c r="J15" s="32"/>
       <c r="K15"/>
-      <c r="L15" s="27"/>
+      <c r="L15" s="32"/>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
     </row>
@@ -843,7 +848,7 @@
       <c r="B16" s="9">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="28" t="s">
@@ -854,10 +859,10 @@
       </c>
       <c r="H16"/>
       <c r="I16" s="19"/>
-      <c r="J16" s="27"/>
+      <c r="J16" s="32"/>
       <c r="K16"/>
       <c r="L16" s="19"/>
-      <c r="M16" s="27"/>
+      <c r="M16" s="32"/>
       <c r="N16" s="19"/>
     </row>
     <row r="17" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -867,7 +872,7 @@
       <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="9">
         <v>0.66666666666666596</v>
       </c>
@@ -876,14 +881,14 @@
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17" s="19"/>
-      <c r="M17" s="27"/>
+      <c r="M17" s="32"/>
       <c r="N17" s="19"/>
     </row>
     <row r="18" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
         <v>0.6875</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="27" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="9">
@@ -893,7 +898,7 @@
       <c r="I18" s="19"/>
       <c r="J18"/>
       <c r="K18"/>
-      <c r="L18" s="27"/>
+      <c r="L18" s="32"/>
       <c r="M18" s="19"/>
       <c r="N18" s="19"/>
     </row>
@@ -901,16 +906,16 @@
       <c r="B19" s="9">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="12"/>
       <c r="E19" s="9">
         <v>0.70833333333333337</v>
       </c>
       <c r="H19"/>
       <c r="I19" s="19"/>
-      <c r="J19" s="27"/>
+      <c r="J19" s="32"/>
       <c r="K19"/>
-      <c r="L19" s="27"/>
+      <c r="L19" s="32"/>
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
     </row>
@@ -918,16 +923,16 @@
       <c r="B20" s="9">
         <v>0.72916666666666663</v>
       </c>
-      <c r="C20" s="25"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="13"/>
       <c r="E20" s="9">
         <v>0.72916666666666663</v>
       </c>
       <c r="H20"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
       <c r="K20"/>
-      <c r="L20" s="27"/>
+      <c r="L20" s="32"/>
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
     </row>
@@ -935,7 +940,7 @@
       <c r="B21" s="9">
         <v>0.75</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="11"/>
@@ -943,10 +948,10 @@
         <v>0.75</v>
       </c>
       <c r="H21"/>
-      <c r="I21" s="27"/>
+      <c r="I21" s="32"/>
       <c r="J21"/>
       <c r="K21"/>
-      <c r="L21" s="27"/>
+      <c r="L21" s="32"/>
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
     </row>
@@ -956,7 +961,7 @@
       <c r="E22" s="18"/>
       <c r="H22"/>
       <c r="I22"/>
-      <c r="J22" s="27"/>
+      <c r="J22" s="32"/>
       <c r="K22"/>
       <c r="L22" s="19"/>
       <c r="M22" s="19"/>
@@ -966,10 +971,10 @@
       <c r="B23" s="1"/>
       <c r="H23"/>
       <c r="I23"/>
-      <c r="J23" s="27"/>
+      <c r="J23" s="32"/>
       <c r="K23"/>
       <c r="L23" s="19"/>
-      <c r="M23" s="27"/>
+      <c r="M23" s="32"/>
       <c r="N23" s="19"/>
     </row>
     <row r="24" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -980,10 +985,10 @@
       <c r="D24" s="15"/>
       <c r="H24"/>
       <c r="I24"/>
-      <c r="J24" s="27"/>
+      <c r="J24" s="32"/>
       <c r="K24"/>
       <c r="L24" s="19"/>
-      <c r="M24" s="27"/>
+      <c r="M24" s="32"/>
       <c r="N24" s="19"/>
     </row>
     <row r="25" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -993,9 +998,9 @@
       </c>
       <c r="D25" s="19"/>
       <c r="I25"/>
-      <c r="J25" s="27"/>
+      <c r="J25" s="32"/>
       <c r="K25"/>
-      <c r="L25" s="27"/>
+      <c r="L25" s="32"/>
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
     </row>
@@ -1006,14 +1011,14 @@
       </c>
       <c r="D26" s="19"/>
       <c r="I26"/>
-      <c r="J26" s="27"/>
+      <c r="J26" s="32"/>
       <c r="K26"/>
-      <c r="L26" s="27"/>
+      <c r="L26" s="32"/>
       <c r="M26" s="19"/>
       <c r="N26" s="19"/>
     </row>
     <row r="27" spans="2:14" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="27"/>
+      <c r="D27" s="32"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -1023,9 +1028,9 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C28" s="14"/>
-      <c r="D28" s="27"/>
+      <c r="D28" s="32"/>
       <c r="I28"/>
-      <c r="J28" s="27"/>
+      <c r="J28" s="32"/>
       <c r="K28"/>
       <c r="L28" s="19"/>
       <c r="M28" s="19"/>
@@ -1033,9 +1038,9 @@
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C29" s="15"/>
-      <c r="D29" s="27"/>
+      <c r="D29" s="32"/>
       <c r="I29"/>
-      <c r="J29" s="27"/>
+      <c r="J29" s="32"/>
       <c r="K29"/>
       <c r="L29" s="19"/>
       <c r="M29" s="19"/>
@@ -1043,28 +1048,28 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C30" s="15"/>
-      <c r="D30" s="27"/>
+      <c r="D30" s="32"/>
       <c r="I30"/>
-      <c r="J30" s="27"/>
+      <c r="J30" s="32"/>
       <c r="K30"/>
       <c r="L30" s="19"/>
-      <c r="M30" s="27"/>
+      <c r="M30" s="32"/>
       <c r="N30" s="19"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C31" s="15"/>
       <c r="I31"/>
-      <c r="J31" s="27"/>
+      <c r="J31" s="32"/>
       <c r="K31"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
       <c r="N31" s="19"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C32" s="15"/>
       <c r="I32"/>
       <c r="J32"/>
-      <c r="L32" s="27"/>
+      <c r="L32" s="32"/>
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
     </row>
@@ -1086,28 +1091,28 @@
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C35" s="15"/>
       <c r="I35"/>
-      <c r="J35" s="27"/>
+      <c r="J35" s="32"/>
       <c r="L35" s="19"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I36"/>
-      <c r="J36" s="27"/>
-      <c r="L36" s="27"/>
+      <c r="J36" s="32"/>
+      <c r="L36" s="32"/>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I37"/>
-      <c r="J37" s="27"/>
-      <c r="L37" s="27"/>
+      <c r="J37" s="32"/>
+      <c r="L37" s="32"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I38"/>
-      <c r="J38" s="27"/>
-      <c r="L38" s="27"/>
+      <c r="J38" s="32"/>
+      <c r="L38" s="32"/>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="L39" s="27"/>
+      <c r="L39" s="32"/>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C41" s="14"/>
@@ -1156,14 +1161,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="L31:L32"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D10:D12"/>
     <mergeCell ref="L36:L39"/>
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="M23:M24"/>
@@ -1177,13 +1181,14 @@
     <mergeCell ref="J22:J26"/>
     <mergeCell ref="I9:I13"/>
     <mergeCell ref="I20:I21"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="L31:L32"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>